<commit_message>
ci: Add debug step to list files
Adds a step to the `unit-test` job to investigate the file structure available in the CI environment. This is to debug a test failure that may be related to missing test data files.
</commit_message>
<xml_diff>
--- a/data/sample2.xlsx
+++ b/data/sample2.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main">
+<workbook xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
   <workbookPr/>
   <sheets>
-    <sheet state="visible" r:id="rId4" name="シート1" sheetId="1"/>
+    <sheet name="シート1" state="visible" r:id="rId4" sheetId="1"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac">
   <fonts count="2">
     <font>
       <sz val="10.0"/>
@@ -40,18 +40,18 @@
     <border/>
   </borders>
   <cellStyleXfs count="1">
-    <xf applyFont="1" fillId="0" borderId="0" fontId="0" numFmtId="0" applyAlignment="1"/>
+    <xf fontId="0" fillId="0" applyFont="1" numFmtId="0" borderId="0" applyAlignment="1"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" borderId="0" fillId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom" readingOrder="0" shrinkToFit="0" wrapText="0"/>
+    <xf fontId="0" applyAlignment="1" borderId="0" applyFont="1" fillId="0" xfId="0" numFmtId="0">
+      <alignment shrinkToFit="0" wrapText="0" readingOrder="0" vertical="bottom"/>
     </xf>
-    <xf fillId="0" fontId="1" applyAlignment="1" numFmtId="0" xfId="0" applyFont="1" borderId="0">
+    <xf applyFont="1" numFmtId="0" xfId="0" fillId="0" applyAlignment="1" borderId="0" fontId="1">
       <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" builtinId="0" xfId="0"/>
+    <cellStyle xfId="0" name="Normal" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
 </styleSheet>
@@ -168,25 +168,25 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:lin scaled="0" ang="5400000"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln cap="flat" cmpd="sng" algn="ctr" w="6350">
+        <a:ln cap="flat" algn="ctr" cmpd="sng" w="6350">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln cmpd="sng" w="12700" algn="ctr" cap="flat">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="12700">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln cap="flat" w="19050" cmpd="sng" algn="ctr">
+        <a:ln w="19050" cmpd="sng" algn="ctr" cap="flat">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -203,7 +203,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw algn="ctr" rotWithShape="0" dir="5400000" dist="19050" blurRad="57150">
+            <a:outerShdw algn="ctr" blurRad="57150" dir="5400000" dist="19050" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -255,17 +255,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mv="urn:schemas-microsoft-com:mac:vml">
+<worksheet xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main">
   <sheetPr>
-    <outlinePr summaryRight="0" summaryBelow="0"/>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" customHeight="1" defaultColWidth="12.63"/>
+  <sheetFormatPr defaultRowHeight="15.75" defaultColWidth="12.63" customHeight="1"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1">
+      <c s="1" r="A1">
         <v>1.0</v>
       </c>
       <c r="B1" s="1">
@@ -273,10 +273,10 @@
       </c>
     </row>
     <row r="2">
-      <c s="1" r="A2">
+      <c r="A2" s="1">
         <v>2.0</v>
       </c>
-      <c r="B2" s="1">
+      <c s="1" r="B2">
         <v>4.0</v>
       </c>
     </row>

</xml_diff>